<commit_message>
added a laderboad excel doc that created the json file
</commit_message>
<xml_diff>
--- a/src/data/dynamic/leaderboard.xlsx
+++ b/src/data/dynamic/leaderboard.xlsx
@@ -5,16 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Repos\gmfc\src\data\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Repos\gmfc\src\data\dynamic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2ABCF7-57EC-4C6B-97D9-BA81FF552D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B6965F-42B7-40DB-971D-07B8DD92DCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="1275" windowWidth="20925" windowHeight="14205" xr2:uid="{8741AE50-06A3-4425-B70E-37017E4B69A0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Leaderboard" sheetId="1" r:id="rId1"/>
+    <sheet name="Participant" sheetId="2" r:id="rId2"/>
+    <sheet name="Course" sheetId="3" r:id="rId3"/>
+    <sheet name="Battery" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="Participants">Participant!$A$2:$A$30</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,18 +42,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
-  <si>
-    <t>a</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Toby</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Ben Hooper</t>
+  </si>
+  <si>
+    <t>Toby Black</t>
+  </si>
+  <si>
+    <t>James Carter</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Trophy Course</t>
+  </si>
+  <si>
+    <t>2S</t>
+  </si>
+  <si>
+    <t>3S</t>
+  </si>
+  <si>
+    <t>4S</t>
+  </si>
+  <si>
+    <t>5S</t>
+  </si>
+  <si>
+    <t>6S</t>
+  </si>
+  <si>
+    <t>Laptime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -74,8 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,27 +487,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B4D0C5-CFC6-4A13-9570-790DE40A2076}">
-  <dimension ref="C3:J7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E2" s="2">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52388436-D811-4737-972F-A35577885F51}">
+          <x14:formula1>
+            <xm:f>Participant!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2 A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54C4E92B-5860-4714-8E28-991F60C3EE10}">
+          <x14:formula1>
+            <xm:f>Course!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD53B953-C178-4B69-937A-C17B9E879A63}">
+          <x14:formula1>
+            <xm:f>Battery!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBD091C-1CEE-4FD2-B9EC-48CC73C785F6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FC7A89-B057-4724-831B-8827901FD059}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J7" t="s">
-        <v>0</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A774EDE-4280-47F5-8E1D-23E1BE4D94C7}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added somr more times
</commit_message>
<xml_diff>
--- a/src/data/dynamic/leaderboard.xlsx
+++ b/src/data/dynamic/leaderboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Repos\gmfc\src\data\dynamic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B6965F-42B7-40DB-971D-07B8DD92DCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B93AAE0-3452-42DB-B978-B255A87567F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1275" windowWidth="20925" windowHeight="14205" xr2:uid="{8741AE50-06A3-4425-B70E-37017E4B69A0}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="9810" windowHeight="15585" xr2:uid="{8741AE50-06A3-4425-B70E-37017E4B69A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Leaderboard" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Ben</t>
   </si>
@@ -108,9 +108,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,17 +484,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B4D0C5-CFC6-4A13-9570-790DE40A2076}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -526,13 +523,47 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3">
-        <v>46023</v>
+        <v>45984.651388888888</v>
       </c>
       <c r="E2" s="2">
-        <v>75</v>
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45984.638194444444</v>
+      </c>
+      <c r="E3" s="2">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45984.61041666667</v>
+      </c>
+      <c r="E4" s="2">
+        <v>19.3</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +575,7 @@
           <x14:formula1>
             <xm:f>Participant!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>A2 A2:A1048576</xm:sqref>
+          <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54C4E92B-5860-4714-8E28-991F60C3EE10}">
           <x14:formula1>

</xml_diff>

<commit_message>
added some more info to league table
</commit_message>
<xml_diff>
--- a/src/data/dynamic/leaderboard.xlsx
+++ b/src/data/dynamic/leaderboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Repos\gmfc\src\data\dynamic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7469C36-D317-4350-8968-44B6E0C9F319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD43C9E-93B9-40B5-AB4A-ED4E0B5A6C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7230" yWindow="1275" windowWidth="20925" windowHeight="14205" xr2:uid="{8741AE50-06A3-4425-B70E-37017E4B69A0}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Ben</t>
   </si>
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B4D0C5-CFC6-4A13-9570-790DE40A2076}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +598,23 @@
       </c>
       <c r="E6" s="2">
         <v>19.010000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3">
+        <v>46024.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>18.809999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>